<commit_message>
Added picture of one Baud displayed on an Oszi
</commit_message>
<xml_diff>
--- a/doc/lux_volt.xlsx
+++ b/doc/lux_volt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomka\Documents\school\automation\LDR_Exercises\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B45E1AD-7A8D-4BFB-83ED-942E02FF9CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F298D04-158C-4828-96BB-F781F7E63AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>LUX</t>
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>Baudrate</t>
+  </si>
+  <si>
+    <t>Baud/s</t>
+  </si>
+  <si>
+    <t>1 Baud</t>
+  </si>
+  <si>
+    <t>0,10417</t>
+  </si>
+  <si>
+    <t>ms</t>
   </si>
 </sst>
 </file>
@@ -120,6 +135,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Volt to LUX</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -196,8 +236,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.0180883639545057E-2"/>
-                  <c:y val="-0.1049475065616798"/>
+                  <c:x val="0.11591835164123003"/>
+                  <c:y val="-0.1729092633054376"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="0.00000000E+00" sourceLinked="0"/>
@@ -311,6 +351,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Voltage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -373,6 +468,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>LUX</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1026,9 +1176,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1344,10 +1494,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1356,7 +1506,7 @@
     <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>540</v>
       </c>
@@ -1372,7 +1522,7 @@
         <v>2.6339999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>245</v>
       </c>
@@ -1380,7 +1530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>100</v>
       </c>
@@ -1388,7 +1538,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>624</v>
       </c>
@@ -1396,6 +1546,28 @@
         <v>2.7</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>9600</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>